<commit_message>
Commit finale, progetto completato
</commit_message>
<xml_diff>
--- a/Process control chart/ProjectFALCONComparedTicketDatas.xlsx
+++ b/Process control chart/ProjectFALCONComparedTicketDatas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matteo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4141C843-9D32-4A54-A3B4-A00DAA0437AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903D4ED0-3FD5-4CF4-AA45-1B508152FA17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12360" yWindow="3240" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectFALCONComparedTicketData" sheetId="1" r:id="rId1"/>
@@ -1207,10 +1207,10 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>17</c:v>
@@ -1264,10 +1264,10 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>46</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>39</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>25</c:v>
@@ -1312,10 +1312,10 @@
                   <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>46</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>39</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>6</c:v>
@@ -1333,10 +1333,10 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>20</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>0</c:v>
@@ -2150,220 +2150,220 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="72"/>
                 <c:pt idx="0">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>87.490849155504151</c:v>
+                  <c:v>87.440813566610188</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4070,8 +4070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4115,11 +4115,11 @@
       </c>
       <c r="D2" s="3">
         <f>C2+3*STDEVA($B$2:$B$73)</f>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E2" s="3">
         <f>C2-3*STDEVA($B$2:$B$73)</f>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F2" s="3">
         <v>0</v>
@@ -4138,11 +4138,11 @@
       </c>
       <c r="D3" s="3">
         <f t="shared" ref="D3:D66" si="1">C3+3*STDEVA($B$2:$B$73)</f>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E3" s="3">
         <f t="shared" ref="E3:E66" si="2">C3-3*STDEVA($B$2:$B$73)</f>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F3" s="3">
         <v>0</v>
@@ -4161,11 +4161,11 @@
       </c>
       <c r="D4" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F4" s="3">
         <v>0</v>
@@ -4184,11 +4184,11 @@
       </c>
       <c r="D5" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F5" s="3">
         <v>0</v>
@@ -4207,11 +4207,11 @@
       </c>
       <c r="D6" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F6" s="3">
         <v>0</v>
@@ -4230,11 +4230,11 @@
       </c>
       <c r="D7" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F7" s="3">
         <v>0</v>
@@ -4253,11 +4253,11 @@
       </c>
       <c r="D8" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F8" s="3">
         <v>0</v>
@@ -4268,7 +4268,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" si="0"/>
@@ -4276,11 +4276,11 @@
       </c>
       <c r="D9" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F9" s="3">
         <v>0</v>
@@ -4291,7 +4291,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" si="0"/>
@@ -4299,11 +4299,11 @@
       </c>
       <c r="D10" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F10" s="3">
         <v>0</v>
@@ -4322,11 +4322,11 @@
       </c>
       <c r="D11" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F11" s="3">
         <v>0</v>
@@ -4345,11 +4345,11 @@
       </c>
       <c r="D12" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F12" s="3">
         <v>0</v>
@@ -4368,11 +4368,11 @@
       </c>
       <c r="D13" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F13" s="3">
         <v>0</v>
@@ -4391,11 +4391,11 @@
       </c>
       <c r="D14" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F14" s="3">
         <v>0</v>
@@ -4414,11 +4414,11 @@
       </c>
       <c r="D15" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F15" s="3">
         <v>0</v>
@@ -4437,11 +4437,11 @@
       </c>
       <c r="D16" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F16" s="3">
         <v>0</v>
@@ -4460,11 +4460,11 @@
       </c>
       <c r="D17" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F17" s="3">
         <v>0</v>
@@ -4483,11 +4483,11 @@
       </c>
       <c r="D18" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E18" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F18" s="3">
         <v>0</v>
@@ -4506,11 +4506,11 @@
       </c>
       <c r="D19" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E19" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F19" s="3">
         <v>0</v>
@@ -4529,11 +4529,11 @@
       </c>
       <c r="D20" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E20" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F20" s="3">
         <v>0</v>
@@ -4552,11 +4552,11 @@
       </c>
       <c r="D21" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E21" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F21" s="3">
         <v>0</v>
@@ -4575,11 +4575,11 @@
       </c>
       <c r="D22" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E22" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F22" s="3">
         <v>0</v>
@@ -4598,11 +4598,11 @@
       </c>
       <c r="D23" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E23" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F23" s="3">
         <v>0</v>
@@ -4621,11 +4621,11 @@
       </c>
       <c r="D24" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E24" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F24" s="3">
         <v>0</v>
@@ -4644,11 +4644,11 @@
       </c>
       <c r="D25" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E25" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F25" s="3">
         <v>0</v>
@@ -4667,11 +4667,11 @@
       </c>
       <c r="D26" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E26" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F26" s="3">
         <v>0</v>
@@ -4690,11 +4690,11 @@
       </c>
       <c r="D27" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E27" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F27" s="3">
         <v>0</v>
@@ -4705,7 +4705,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="3">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28" s="3">
         <f t="shared" si="0"/>
@@ -4713,11 +4713,11 @@
       </c>
       <c r="D28" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E28" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F28" s="3">
         <v>0</v>
@@ -4728,7 +4728,7 @@
         <v>66</v>
       </c>
       <c r="B29" s="3">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C29" s="3">
         <f t="shared" si="0"/>
@@ -4736,11 +4736,11 @@
       </c>
       <c r="D29" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E29" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F29" s="3">
         <v>0</v>
@@ -4759,11 +4759,11 @@
       </c>
       <c r="D30" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E30" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F30" s="3">
         <v>0</v>
@@ -4782,11 +4782,11 @@
       </c>
       <c r="D31" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E31" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F31" s="3">
         <v>0</v>
@@ -4805,11 +4805,11 @@
       </c>
       <c r="D32" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E32" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F32" s="3">
         <v>0</v>
@@ -4828,11 +4828,11 @@
       </c>
       <c r="D33" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E33" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F33" s="3">
         <v>0</v>
@@ -4851,11 +4851,11 @@
       </c>
       <c r="D34" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E34" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F34" s="3">
         <v>0</v>
@@ -4874,11 +4874,11 @@
       </c>
       <c r="D35" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E35" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F35" s="3">
         <v>0</v>
@@ -4897,11 +4897,11 @@
       </c>
       <c r="D36" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E36" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F36" s="3">
         <v>0</v>
@@ -4920,11 +4920,11 @@
       </c>
       <c r="D37" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E37" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F37" s="3">
         <v>0</v>
@@ -4943,11 +4943,11 @@
       </c>
       <c r="D38" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E38" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F38" s="3">
         <v>0</v>
@@ -4966,11 +4966,11 @@
       </c>
       <c r="D39" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E39" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F39" s="3">
         <v>0</v>
@@ -4989,11 +4989,11 @@
       </c>
       <c r="D40" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E40" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F40" s="3">
         <v>0</v>
@@ -5012,11 +5012,11 @@
       </c>
       <c r="D41" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E41" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F41" s="3">
         <v>0</v>
@@ -5035,11 +5035,11 @@
       </c>
       <c r="D42" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E42" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F42" s="3">
         <v>0</v>
@@ -5058,11 +5058,11 @@
       </c>
       <c r="D43" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E43" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F43" s="3">
         <v>0</v>
@@ -5073,7 +5073,7 @@
         <v>37</v>
       </c>
       <c r="B44" s="3">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C44" s="3">
         <f t="shared" si="0"/>
@@ -5081,11 +5081,11 @@
       </c>
       <c r="D44" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E44" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F44" s="3">
         <v>0</v>
@@ -5096,7 +5096,7 @@
         <v>38</v>
       </c>
       <c r="B45" s="3">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C45" s="3">
         <f t="shared" si="0"/>
@@ -5104,11 +5104,11 @@
       </c>
       <c r="D45" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E45" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F45" s="3">
         <v>0</v>
@@ -5127,11 +5127,11 @@
       </c>
       <c r="D46" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E46" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F46" s="3">
         <v>0</v>
@@ -5150,11 +5150,11 @@
       </c>
       <c r="D47" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E47" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F47" s="3">
         <v>0</v>
@@ -5173,11 +5173,11 @@
       </c>
       <c r="D48" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E48" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F48" s="3">
         <v>0</v>
@@ -5196,11 +5196,11 @@
       </c>
       <c r="D49" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E49" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F49" s="3">
         <v>0</v>
@@ -5219,11 +5219,11 @@
       </c>
       <c r="D50" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E50" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F50" s="3">
         <v>0</v>
@@ -5234,7 +5234,7 @@
         <v>43</v>
       </c>
       <c r="B51" s="3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C51" s="3">
         <f t="shared" si="0"/>
@@ -5242,11 +5242,11 @@
       </c>
       <c r="D51" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E51" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F51" s="3">
         <v>0</v>
@@ -5257,7 +5257,7 @@
         <v>44</v>
       </c>
       <c r="B52" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C52" s="3">
         <f t="shared" si="0"/>
@@ -5265,11 +5265,11 @@
       </c>
       <c r="D52" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E52" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F52" s="3">
         <v>0</v>
@@ -5288,11 +5288,11 @@
       </c>
       <c r="D53" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E53" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F53" s="3">
         <v>0</v>
@@ -5311,11 +5311,11 @@
       </c>
       <c r="D54" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E54" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F54" s="3">
         <v>0</v>
@@ -5334,11 +5334,11 @@
       </c>
       <c r="D55" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E55" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F55" s="3">
         <v>0</v>
@@ -5357,11 +5357,11 @@
       </c>
       <c r="D56" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E56" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F56" s="3">
         <v>0</v>
@@ -5380,11 +5380,11 @@
       </c>
       <c r="D57" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E57" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F57" s="3">
         <v>0</v>
@@ -5403,11 +5403,11 @@
       </c>
       <c r="D58" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E58" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F58" s="3">
         <v>0</v>
@@ -5426,11 +5426,11 @@
       </c>
       <c r="D59" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E59" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F59" s="3">
         <v>0</v>
@@ -5449,11 +5449,11 @@
       </c>
       <c r="D60" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E60" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F60" s="3">
         <v>0</v>
@@ -5472,11 +5472,11 @@
       </c>
       <c r="D61" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E61" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F61" s="3">
         <v>0</v>
@@ -5495,11 +5495,11 @@
       </c>
       <c r="D62" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E62" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F62" s="3">
         <v>0</v>
@@ -5518,11 +5518,11 @@
       </c>
       <c r="D63" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E63" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F63" s="3">
         <v>0</v>
@@ -5541,11 +5541,11 @@
       </c>
       <c r="D64" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E64" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F64" s="3">
         <v>0</v>
@@ -5564,11 +5564,11 @@
       </c>
       <c r="D65" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E65" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F65" s="3">
         <v>0</v>
@@ -5587,11 +5587,11 @@
       </c>
       <c r="D66" s="3">
         <f t="shared" si="1"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E66" s="3">
         <f t="shared" si="2"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F66" s="3">
         <v>0</v>
@@ -5610,11 +5610,11 @@
       </c>
       <c r="D67" s="3">
         <f t="shared" ref="D67:D73" si="4">C67+3*STDEVA($B$2:$B$73)</f>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E67" s="3">
         <f t="shared" ref="E67:E73" si="5">C67-3*STDEVA($B$2:$B$73)</f>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F67" s="3">
         <v>0</v>
@@ -5633,11 +5633,11 @@
       </c>
       <c r="D68" s="3">
         <f t="shared" si="4"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E68" s="3">
         <f t="shared" si="5"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F68" s="3">
         <v>0</v>
@@ -5656,11 +5656,11 @@
       </c>
       <c r="D69" s="3">
         <f t="shared" si="4"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E69" s="3">
         <f t="shared" si="5"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F69" s="3">
         <v>0</v>
@@ -5679,11 +5679,11 @@
       </c>
       <c r="D70" s="3">
         <f t="shared" si="4"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E70" s="3">
         <f t="shared" si="5"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F70" s="3">
         <v>0</v>
@@ -5702,11 +5702,11 @@
       </c>
       <c r="D71" s="3">
         <f t="shared" si="4"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E71" s="3">
         <f t="shared" si="5"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F71" s="3">
         <v>0</v>
@@ -5725,11 +5725,11 @@
       </c>
       <c r="D72" s="3">
         <f t="shared" si="4"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E72" s="3">
         <f t="shared" si="5"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F72" s="3">
         <v>0</v>
@@ -5748,11 +5748,11 @@
       </c>
       <c r="D73" s="3">
         <f t="shared" si="4"/>
-        <v>87.490849155504151</v>
+        <v>87.440813566610188</v>
       </c>
       <c r="E73" s="3">
         <f t="shared" si="5"/>
-        <v>-44.296404711059701</v>
+        <v>-44.246369122165738</v>
       </c>
       <c r="F73" s="3">
         <v>0</v>

</xml_diff>